<commit_message>
docs: 돌진패턴 duration 값 수정 2차
</commit_message>
<xml_diff>
--- a/DragAndDrop/Assets/5.Data/Cloud_rush_data-1.0.xlsx
+++ b/DragAndDrop/Assets/5.Data/Cloud_rush_data-1.0.xlsx
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -837,18 +837,18 @@
         <v>4</v>
       </c>
       <c r="C36">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>43.5</v>
+        <v>43.75</v>
       </c>
       <c r="B37" s="1">
         <v>4</v>
       </c>
       <c r="C37">
-        <v>0.55000000000000004</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>